<commit_message>
Add Download Monthly Report
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Evan\2-TestGitHub\1-UiPath\GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393D04AC-19EA-4487-ABAD-077B12D75EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97B01C6-9E0A-4C90-8358-6FC3241B9828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>GenerateYearlyReportQueue</t>
   </si>
   <si>
-    <t>ACME_URL</t>
-  </si>
-  <si>
     <t>ACME_Credential</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
   </si>
   <si>
     <t>WI4</t>
-  </si>
-  <si>
-    <t>ACME_WorkItemDetails_URL</t>
   </si>
   <si>
     <t>https://acme-test.uipath.com/work-items/</t>
@@ -231,6 +225,14 @@
   </si>
   <si>
     <t>ACME Upload Yearly Report page has not found.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ACME_URL</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ACME_WorkItemDetails_URL</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -616,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -689,93 +691,109 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>33</v>
+      <c r="A6" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>52</v>
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>48</v>
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="5"/>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1740,13 +1758,16 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{5CA192EE-8A69-4594-8E7A-1A1989EEE8FB}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{DE67080B-75CD-4D66-95BE-30145F56FD3B}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{12F88D01-72F3-4173-8CB9-F9B7F64AA46A}"/>
-    <hyperlink ref="B9" r:id="rId4" xr:uid="{532A78DD-3749-4F0F-8372-065304387BE5}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{DE67080B-75CD-4D66-95BE-30145F56FD3B}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{12F88D01-72F3-4173-8CB9-F9B7F64AA46A}"/>
+    <hyperlink ref="B12" r:id="rId4" xr:uid="{532A78DD-3749-4F0F-8372-065304387BE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -1757,7 +1778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1884,40 +1905,40 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
         <v>42</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2954,13 +2975,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Finish ExtractWorkItems and RetrieveTaxId
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Evan\2-TestGitHub\1-UiPath\GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97B01C6-9E0A-4C90-8358-6FC3241B9828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B1A597-C308-4250-8CD3-4DC16AEA16FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -135,9 +135,6 @@
     <t>No ACME_URL value in Settings sheet</t>
   </si>
   <si>
-    <t>My Workspace</t>
-  </si>
-  <si>
     <t>ExtractWorkItemTypeName</t>
   </si>
   <si>
@@ -160,10 +157,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>"Create New Queue Items in Queue Name: {0},  values are TaxID: {1},Name: {2} and Address: {3}."</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>ACME_Credential</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -233,6 +226,18 @@
   </si>
   <si>
     <t>ACME_WorkItemDetails_URL</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LogMessage_Add_New_QueueItem_Already_Existed</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Create New Queue Items in Queue Name: {0},  values are TaxID: {1},Name: {2} and Address: {3}.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Queue Items in Queue Name: {0},  values are TaxID: {1},Name: {2} and Address: {3} already in Queues.</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -251,6 +256,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -269,6 +275,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -620,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -692,13 +699,13 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -708,13 +715,13 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -724,10 +731,10 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -736,10 +743,10 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -752,38 +759,45 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1778,14 +1792,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="58.85546875" customWidth="1"/>
+    <col min="2" max="2" width="100.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -1905,7 +1919,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
@@ -1916,32 +1930,39 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -2926,7 +2947,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2973,19 +2994,12 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3985,5 +3999,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Test case for Download Monthly Report
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Evan\2-TestGitHub\1-UiPath\GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B1A597-C308-4250-8CD3-4DC16AEA16FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33117D00-77B6-448E-B266-214D08E6CD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -120,9 +120,6 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>https://acme-test.uipath.com/</t>
-  </si>
-  <si>
     <t>GenerateYearlyReportQueue</t>
   </si>
   <si>
@@ -238,6 +235,10 @@
   </si>
   <si>
     <t>Queue Items in Queue Name: {0},  values are TaxID: {1},Name: {2} and Address: {3} already in Queues.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -627,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -678,7 +679,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -699,13 +700,13 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -715,13 +716,13 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -731,10 +732,10 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -743,10 +744,10 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -759,43 +760,43 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1792,7 +1793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1919,48 +1920,48 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Finished Download Monthly Report process
Loop download monthly report from January to December and also add log if no report for this month
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Evan\2-TestGitHub\1-UiPath\GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33117D00-77B6-448E-B266-214D08E6CD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8704B0D-EBCD-46A9-BD86-395021421D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>https://acme-test.uipath.com/work-items/</t>
   </si>
   <si>
-    <t>LogMessage_BusinessRuleException_No_Data</t>
-  </si>
-  <si>
     <t>{0} month has no report</t>
   </si>
   <si>
@@ -239,6 +236,10 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>LogMessage_BusinessRuleException_No_Data</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -628,7 +629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -700,13 +701,13 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -716,13 +717,13 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -732,10 +733,10 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -744,10 +745,10 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -766,34 +767,34 @@
         <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
@@ -1793,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1920,7 +1921,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -1930,38 +1931,38 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add Update Work Item
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Evan\2-TestGitHub\1-UiPath\GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81DE5F2-2E03-41F8-B7B0-05B41BE3B311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6E862B-94FD-42AD-84FF-BB8A59805433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,9 +131,6 @@
     <t>ExtractWorkItemTypeName</t>
   </si>
   <si>
-    <t>https://acme-test.uipath.com/work-items/</t>
-  </si>
-  <si>
     <t>{0} month has no report</t>
   </si>
   <si>
@@ -255,6 +252,10 @@
   <si>
     <t>Orchestrator queue Name in "My Workspace". Please also set "Uniqueue Reference" option to Yes, because we will use TaxId as Uniqueue Reference. The value must match with the queue name defined on Orchestrator.
 After you first created the Queue name, please wait about 1 minutes before run it, it has a delay duration when RPA app to call it.</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items/</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -643,7 +644,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -696,7 +697,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -714,13 +715,13 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -730,13 +731,13 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -746,10 +747,10 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -758,10 +759,10 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -777,37 +778,37 @@
         <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
         <v>31</v>
@@ -816,13 +817,13 @@
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1944,7 +1945,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
@@ -1955,37 +1956,37 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
         <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>